<commit_message>
Adding order, order processor, file handler
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -5,14 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCIT\CST\COMP 3 V (Prog Paradigms)\COMP3522 Object Oriented Programming 2 6.0\Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCIT\CST\COMP 3 V (Prog Paradigms)\COMP3522 Object Oriented Programming 2 6.0\COMP3522_Assignment2_A01054885_A01005378\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5895"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5895" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="131">
   <si>
     <t>name</t>
   </si>
@@ -306,13 +308,189 @@
   </si>
   <si>
     <t>Sea Salt</t>
+  </si>
+  <si>
+    <t>item</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>common property</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>specific property</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>holiday</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Toy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>order_number</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Santa's Workshop
+(C____T)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>dimensions (width, height)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Christmas</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>num_rooms</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RC (Remote Controlled) Spider
+(H____T)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halloween</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halloween</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_glow (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>spider_type
+(Tarantula/Wolf Spider)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Robot Bunny
+(E____T)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Easter</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_batteries (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>colour
+(Orange/Blue/Pink)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Stuffed Animal</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dancing Skeleton
+(H____S)
+(Acrylic &amp; Polyester Fiberfill)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_glow (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Halloween</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reindeer
+(C____S)
+(Cotton &amp; Wool)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_glow (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>stuffing
+(Polyester Fiberfill/Wool)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Easter Bunny 
+(E____S)
+(Linen &amp; Polyester Fiberfill)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>colour
+(White/Grey/Pink/Blue)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>size
+(S/M/L)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>fabric
+(Acrylic/Cotton/Linen)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Candy</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pumpkin Caramel Toffee
+(H____C)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>variety
+(Sea Salt/Regular)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Candy Canes
+(C____C)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>colour
+(Red/Green)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Creme Eggs
+(E____C)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_lactose (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>has_nuts (Y/N)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +505,13 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -336,7 +521,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -344,14 +529,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -669,9 +937,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T14" sqref="T14"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1280,4 +1548,1445 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:F30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="2" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="11"/>
+      <c r="C4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="11"/>
+      <c r="C5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="11"/>
+      <c r="C6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11"/>
+      <c r="E6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="11"/>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7" s="11"/>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="11"/>
+      <c r="E7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="11"/>
+    </row>
+    <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B8" s="11"/>
+      <c r="C8" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="11"/>
+      <c r="E8" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8" s="11"/>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9" s="11"/>
+      <c r="C9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="11"/>
+      <c r="C10" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D10" s="11"/>
+      <c r="E10" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10" s="11"/>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11" s="11"/>
+      <c r="C11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="F11" s="11"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B13" s="11"/>
+      <c r="C13" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B14" s="11"/>
+      <c r="C14" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" s="12"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B15" s="11"/>
+      <c r="C15" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="12"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="11"/>
+      <c r="C17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="12"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18" s="11"/>
+      <c r="C18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="12"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+    </row>
+    <row r="19" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B19" s="11"/>
+      <c r="C19" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="11"/>
+    </row>
+    <row r="21" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+      <c r="B21" s="11"/>
+      <c r="C21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23" s="11"/>
+      <c r="C23" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24" s="11"/>
+      <c r="C24" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="11"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25" s="11"/>
+      <c r="C25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="11"/>
+      <c r="C26" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="11"/>
+      <c r="C27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="11"/>
+      <c r="C28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="11"/>
+      <c r="C29" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D29" s="12"/>
+      <c r="E29" s="11"/>
+      <c r="F29" s="11"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="11"/>
+      <c r="C30" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D30" s="12"/>
+      <c r="E30" s="11"/>
+      <c r="F30" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="B12:B21"/>
+    <mergeCell ref="D12:D15"/>
+    <mergeCell ref="E12:E15"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="D19:D21"/>
+    <mergeCell ref="E19:E21"/>
+    <mergeCell ref="F19:F21"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="F28:F30"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.75" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.25" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="9" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="10">
+        <v>10</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="10">
+        <v>5</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="10">
+        <v>5</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="10">
+        <v>4</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="10">
+        <v>10</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
+      <c r="J6" s="10">
+        <v>30</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A8" s="10">
+        <v>5</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="10">
+        <v>9</v>
+      </c>
+      <c r="J8" s="10">
+        <v>11</v>
+      </c>
+      <c r="K8" s="10">
+        <v>3</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A10" s="10">
+        <v>11</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="10">
+        <v>4</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="10">
+        <v>9</v>
+      </c>
+      <c r="J10" s="10">
+        <v>15</v>
+      </c>
+      <c r="K10" s="10">
+        <v>5</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A12" s="10">
+        <v>12</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="10">
+        <v>1</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I12" s="10">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10">
+        <v>4</v>
+      </c>
+      <c r="K12" s="10">
+        <v>1</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A14" s="10">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="10">
+        <v>2</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+      <c r="A16" s="10">
+        <v>7</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="E16" s="10">
+        <v>1</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A18" s="10">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="K19" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A20" s="10">
+        <v>10</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="10">
+        <v>5</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="I20" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K20" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H21" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I21" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="10">
+        <v>9</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E22" s="10">
+        <v>6</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="I22" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H23" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
+        <v>6</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I24" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J24" s="10">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="I25" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
+        <v>13</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E26" s="10">
+        <v>10</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="H27" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="A28" s="10">
+        <v>14</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="10">
+        <v>13</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I28" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="G31" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refined menu and added error checking for invalid orders
</commit_message>
<xml_diff>
--- a/orders.xlsx
+++ b/orders.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BCIT\CST\COMP 3 V (Prog Paradigms)\COMP3522 Object Oriented Programming 2 6.0\COMP3522_Assignment2_A01054885_A01005378\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicky\PycharmProjects\COMP3522_Assignment2_A01054885_A01005378\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AEBDFA-83D7-4642-816C-1550AA393F19}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="5895" activeTab="2"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -489,25 +490,25 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -623,7 +624,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -934,37 +935,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="1" max="1" width="17.73046875" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="33.25" customWidth="1"/>
+    <col min="4" max="4" width="33.265625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="15.875" customWidth="1"/>
-    <col min="7" max="7" width="56.875" customWidth="1"/>
+    <col min="6" max="6" width="15.86328125" customWidth="1"/>
+    <col min="7" max="7" width="56.86328125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="9.625" customWidth="1"/>
-    <col min="10" max="10" width="14.375" customWidth="1"/>
-    <col min="11" max="11" width="12.875" customWidth="1"/>
-    <col min="13" max="13" width="13.25" customWidth="1"/>
-    <col min="14" max="14" width="10.125" customWidth="1"/>
-    <col min="15" max="15" width="14.875" customWidth="1"/>
-    <col min="16" max="16" width="13.375" customWidth="1"/>
-    <col min="17" max="17" width="8.375" customWidth="1"/>
-    <col min="18" max="18" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="9.59765625" customWidth="1"/>
+    <col min="10" max="10" width="14.3984375" customWidth="1"/>
+    <col min="11" max="11" width="12.86328125" customWidth="1"/>
+    <col min="13" max="13" width="13.265625" customWidth="1"/>
+    <col min="14" max="14" width="10.1328125" customWidth="1"/>
+    <col min="15" max="15" width="14.86328125" customWidth="1"/>
+    <col min="16" max="16" width="13.3984375" customWidth="1"/>
+    <col min="17" max="17" width="8.3984375" customWidth="1"/>
+    <col min="18" max="18" width="12.59765625" customWidth="1"/>
     <col min="22" max="22" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1073,7 +1074,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" ht="28.5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1108,7 +1109,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="28.5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="28.5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1219,7 +1220,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1251,7 +1252,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" ht="28.5">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1286,7 +1287,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" ht="28.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1353,7 +1354,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" ht="28.5">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" ht="28.5">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1429,7 +1430,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="28.5">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1470,7 +1471,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1502,7 +1503,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:24" ht="33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" ht="28.5">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1534,13 +1535,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24">
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="7:7">
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="7:7">
       <c r="G18" s="1"/>
     </row>
   </sheetData>
@@ -1551,26 +1552,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:F30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="2" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="29.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.75" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.86328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="29.86328125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.73046875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:6" ht="11.25" customHeight="1"/>
+    <row r="2" spans="2:6">
       <c r="B2" s="3" t="s">
         <v>92</v>
       </c>
@@ -1587,7 +1588,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6">
       <c r="B3" s="11" t="s">
         <v>97</v>
       </c>
@@ -1604,7 +1605,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6">
       <c r="B4" s="11"/>
       <c r="C4" s="5" t="s">
         <v>1</v>
@@ -1615,7 +1616,7 @@
       </c>
       <c r="F4" s="11"/>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6">
       <c r="B5" s="11"/>
       <c r="C5" s="5" t="s">
         <v>2</v>
@@ -1630,7 +1631,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6">
       <c r="B6" s="11"/>
       <c r="C6" s="5" t="s">
         <v>0</v>
@@ -1641,7 +1642,7 @@
       </c>
       <c r="F6" s="11"/>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6">
       <c r="B7" s="11"/>
       <c r="C7" s="5" t="s">
         <v>3</v>
@@ -1652,7 +1653,7 @@
       </c>
       <c r="F7" s="11"/>
     </row>
-    <row r="8" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" ht="28.5">
       <c r="B8" s="11"/>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -1663,7 +1664,7 @@
       </c>
       <c r="F8" s="11"/>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6">
       <c r="B9" s="11"/>
       <c r="C9" s="5" t="s">
         <v>7</v>
@@ -1678,7 +1679,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="28.5">
       <c r="B10" s="11"/>
       <c r="C10" s="5" t="s">
         <v>110</v>
@@ -1689,7 +1690,7 @@
       </c>
       <c r="F10" s="11"/>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:6">
       <c r="B11" s="11"/>
       <c r="C11" s="6" t="s">
         <v>6</v>
@@ -1697,7 +1698,7 @@
       <c r="D11" s="11"/>
       <c r="F11" s="11"/>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6">
       <c r="B12" s="11" t="s">
         <v>112</v>
       </c>
@@ -1714,7 +1715,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:6">
       <c r="B13" s="11"/>
       <c r="C13" s="5" t="s">
         <v>1</v>
@@ -1723,7 +1724,7 @@
       <c r="E13" s="11"/>
       <c r="F13" s="11"/>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:6">
       <c r="B14" s="11"/>
       <c r="C14" s="5" t="s">
         <v>2</v>
@@ -1732,7 +1733,7 @@
       <c r="E14" s="11"/>
       <c r="F14" s="11"/>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:6">
       <c r="B15" s="11"/>
       <c r="C15" s="5" t="s">
         <v>0</v>
@@ -1741,7 +1742,7 @@
       <c r="E15" s="11"/>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:6">
       <c r="B16" s="11"/>
       <c r="C16" s="5" t="s">
         <v>3</v>
@@ -1756,7 +1757,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6">
       <c r="B17" s="11"/>
       <c r="C17" s="5" t="s">
         <v>4</v>
@@ -1765,7 +1766,7 @@
       <c r="E17" s="11"/>
       <c r="F17" s="11"/>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6">
       <c r="B18" s="11"/>
       <c r="C18" s="5" t="s">
         <v>7</v>
@@ -1774,7 +1775,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="11"/>
     </row>
-    <row r="19" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="28.5">
       <c r="B19" s="11"/>
       <c r="C19" s="9" t="s">
         <v>118</v>
@@ -1789,7 +1790,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="28.5">
       <c r="B20" s="11"/>
       <c r="C20" s="9" t="s">
         <v>121</v>
@@ -1798,7 +1799,7 @@
       <c r="E20" s="12"/>
       <c r="F20" s="11"/>
     </row>
-    <row r="21" spans="2:6" ht="33" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="28.5">
       <c r="B21" s="11"/>
       <c r="C21" s="7" t="s">
         <v>122</v>
@@ -1807,7 +1808,7 @@
       <c r="E21" s="12"/>
       <c r="F21" s="11"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6">
       <c r="B22" s="11" t="s">
         <v>123</v>
       </c>
@@ -1824,7 +1825,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6">
       <c r="B23" s="11"/>
       <c r="C23" s="5" t="s">
         <v>1</v>
@@ -1833,7 +1834,7 @@
       <c r="E23" s="12"/>
       <c r="F23" s="11"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6">
       <c r="B24" s="11"/>
       <c r="C24" s="5" t="s">
         <v>2</v>
@@ -1842,7 +1843,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="11"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6">
       <c r="B25" s="11"/>
       <c r="C25" s="5" t="s">
         <v>0</v>
@@ -1857,7 +1858,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6">
       <c r="B26" s="11"/>
       <c r="C26" s="5" t="s">
         <v>3</v>
@@ -1866,7 +1867,7 @@
       <c r="E26" s="12"/>
       <c r="F26" s="11"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6">
       <c r="B27" s="11"/>
       <c r="C27" s="5" t="s">
         <v>4</v>
@@ -1875,7 +1876,7 @@
       <c r="E27" s="12"/>
       <c r="F27" s="11"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6">
       <c r="B28" s="11"/>
       <c r="C28" s="5" t="s">
         <v>7</v>
@@ -1890,7 +1891,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6">
       <c r="B29" s="11"/>
       <c r="C29" s="5" t="s">
         <v>129</v>
@@ -1899,7 +1900,7 @@
       <c r="E29" s="11"/>
       <c r="F29" s="11"/>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6">
       <c r="B30" s="11"/>
       <c r="C30" s="6" t="s">
         <v>130</v>
@@ -1910,13 +1911,16 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="D5:D8"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="F9:F11"/>
+    <mergeCell ref="B22:B30"/>
+    <mergeCell ref="D22:D24"/>
+    <mergeCell ref="E22:E24"/>
+    <mergeCell ref="F22:F24"/>
+    <mergeCell ref="D25:D27"/>
+    <mergeCell ref="E25:E27"/>
+    <mergeCell ref="F25:F27"/>
+    <mergeCell ref="D28:D30"/>
+    <mergeCell ref="E28:E30"/>
+    <mergeCell ref="F28:F30"/>
     <mergeCell ref="B12:B21"/>
     <mergeCell ref="D12:D15"/>
     <mergeCell ref="E12:E15"/>
@@ -1927,16 +1931,13 @@
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="E19:E21"/>
     <mergeCell ref="F19:F21"/>
-    <mergeCell ref="B22:B30"/>
-    <mergeCell ref="D22:D24"/>
-    <mergeCell ref="E22:E24"/>
-    <mergeCell ref="F22:F24"/>
-    <mergeCell ref="D25:D27"/>
-    <mergeCell ref="E25:E27"/>
-    <mergeCell ref="F25:F27"/>
-    <mergeCell ref="D28:D30"/>
-    <mergeCell ref="E28:E30"/>
-    <mergeCell ref="F28:F30"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="F9:F11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1945,43 +1946,43 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="13.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.46484375" style="10" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.5" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.875" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.125" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.75" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.25" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.375" style="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="4.625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.46484375" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.86328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1328125" style="10" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.73046875" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.265625" style="10" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.3984375" style="10" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.59765625" style="10" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.3984375" style="10" bestFit="1" customWidth="1"/>
     <col min="25" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13">
       <c r="A1" s="10" t="s">
         <v>16</v>
       </c>
@@ -2016,7 +2017,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="10">
         <v>1</v>
       </c>
@@ -2051,7 +2052,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="A3" s="10" t="s">
         <v>16</v>
       </c>
@@ -2086,7 +2087,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="28.5">
       <c r="A4" s="10">
         <v>3</v>
       </c>
@@ -2121,7 +2122,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="A5" s="10" t="s">
         <v>16</v>
       </c>
@@ -2156,7 +2157,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -2191,7 +2192,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="28.5">
       <c r="A8" s="10">
         <v>5</v>
       </c>
@@ -2273,7 +2274,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="A9" s="10" t="s">
         <v>16</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="28.5">
       <c r="A10" s="10">
         <v>11</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="A11" s="10" t="s">
         <v>16</v>
       </c>
@@ -2396,7 +2397,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="28.5">
       <c r="A12" s="10">
         <v>12</v>
       </c>
@@ -2437,7 +2438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="A13" s="10" t="s">
         <v>16</v>
       </c>
@@ -2472,7 +2473,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="28.5">
       <c r="A14" s="10">
         <v>2</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="A15" s="10" t="s">
         <v>16</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="28.5">
       <c r="A16" s="10">
         <v>7</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11">
       <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
@@ -2612,7 +2613,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="28.5">
       <c r="A18" s="10">
         <v>8</v>
       </c>
@@ -2647,7 +2648,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11">
       <c r="A19" s="10" t="s">
         <v>16</v>
       </c>
@@ -2682,7 +2683,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="28.5">
       <c r="A20" s="10">
         <v>10</v>
       </c>
@@ -2717,7 +2718,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11">
       <c r="A21" s="10" t="s">
         <v>16</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11">
       <c r="A22" s="10">
         <v>9</v>
       </c>
@@ -2781,7 +2782,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11">
       <c r="A23" s="10" t="s">
         <v>16</v>
       </c>
@@ -2813,7 +2814,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11">
       <c r="A24" s="10">
         <v>6</v>
       </c>
@@ -2845,7 +2846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11">
       <c r="A25" s="10" t="s">
         <v>16</v>
       </c>
@@ -2880,7 +2881,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11">
       <c r="A26" s="10">
         <v>13</v>
       </c>
@@ -2912,7 +2913,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11">
       <c r="A27" s="10" t="s">
         <v>16</v>
       </c>
@@ -2944,7 +2945,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="33" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="28.5">
       <c r="A28" s="10">
         <v>14</v>
       </c>
@@ -2976,13 +2977,13 @@
         <v>91</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11">
       <c r="G31" s="1"/>
     </row>
   </sheetData>

</xml_diff>